<commit_message>
Attempted yml fix (4)
</commit_message>
<xml_diff>
--- a/resources/rules.xlsx
+++ b/resources/rules.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tazvongpatarakul/Desktop/CodingStuff/Email Bot/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E1619C-70A9-2742-AAA5-E88DB7B95EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30BC280-0DA8-8949-9090-2FE7E67422D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34200" windowHeight="21380" activeTab="1" xr2:uid="{BF4DFA8F-5AC1-D046-ABB2-A830C2A778D3}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34200" windowHeight="21380" xr2:uid="{BF4DFA8F-5AC1-D046-ABB2-A830C2A778D3}"/>
   </bookViews>
   <sheets>
     <sheet name="MainSheet" sheetId="1" r:id="rId1"/>
     <sheet name="ClearanceRules" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Untitled" localSheetId="1">ClearanceRules!$A$8:$A$59</definedName>
+    <definedName name="Untitled" localSheetId="1">ClearanceRules!$A$8:$A$60</definedName>
     <definedName name="Untitled" localSheetId="0">MainSheet!$A$11:$A$62</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -887,9 +887,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC45E019-7CC8-274F-A9ED-A4C3808BD8E0}">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2:P7"/>
+      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1134,7 +1134,7 @@
         <v>14</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="L6" s="7" t="s">
         <v>24</v>
@@ -1552,8 +1552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4EFEE91-1E18-C948-9AD9-53AACE0C2C3C}">
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:P5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1770,7 +1770,7 @@
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
     </row>
-    <row r="6" spans="1:18" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>67</v>
       </c>
@@ -1884,12 +1884,12 @@
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
     </row>
-    <row r="9" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="136" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>16</v>
@@ -1901,7 +1901,7 @@
         <v>38</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>14</v>
@@ -1913,7 +1913,7 @@
         <v>20</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="M9" s="10"/>
       <c r="N9" s="11"/>
@@ -1924,10 +1924,10 @@
     </row>
     <row r="10" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>16</v>
@@ -1936,10 +1936,10 @@
         <v>18</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>14</v>
@@ -1960,24 +1960,24 @@
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
     </row>
-    <row r="11" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>18</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>14</v>
@@ -1989,7 +1989,7 @@
         <v>20</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="M11" s="10"/>
       <c r="N11" s="11"/>
@@ -1998,24 +1998,24 @@
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
     </row>
-    <row r="12" spans="1:18" ht="136" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>18</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>14</v>
@@ -2027,7 +2027,7 @@
         <v>20</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>30</v>
+        <v>94</v>
       </c>
       <c r="M12" s="10"/>
       <c r="N12" s="11"/>
@@ -2153,10 +2153,10 @@
     <mergeCell ref="M2:P5"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G13:G1048576 I13:I1048576 G5:G8 I5:I8 E5:E8 I11 G11 E11 E13:E1048576" xr:uid="{B85A1B20-9ADE-0D41-A64A-493408EBBBE8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G14:G1048576 I14:I1048576 I12 G12 E12 E14:E1048576 I5:I8 E5:E8 G5:G8" xr:uid="{B85A1B20-9ADE-0D41-A64A-493408EBBBE8}">
       <formula1>"None, Sender, Subject, Body, Date, Important, Tag, Attachment"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I4 G2:G4 E2:E4 I9:I10 G9:G10 E9:E10 E12 G12 I12" xr:uid="{8B2A8305-DAE6-FF47-8A35-6C536F794DDE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I4 G2:G4 E2:E4 I9:I11 G9:G11 E9:E11 E13 G13 I13" xr:uid="{8B2A8305-DAE6-FF47-8A35-6C536F794DDE}">
       <formula1>"None, Sender, Subject, Body, Date, Important, Tag, Attachment, Replies"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{B2736DE1-0E25-024A-903B-3527F7C3707B}">

</xml_diff>

<commit_message>
Edited excel sheet (2)
</commit_message>
<xml_diff>
--- a/resources/rules.xlsx
+++ b/resources/rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tazvongpatarakul/Desktop/CodingStuff/Email Bot/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3016482-32CE-424B-81DD-88E2FED32101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4CE6A7-0A57-5E44-9E07-D92420293BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34200" windowHeight="21380" xr2:uid="{BF4DFA8F-5AC1-D046-ABB2-A830C2A778D3}"/>
   </bookViews>
@@ -891,8 +891,8 @@
   <dimension ref="A1:R31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L16" sqref="L16"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1236,7 +1236,7 @@
         <v>28</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>38</v>
@@ -1251,7 +1251,7 @@
         <v>14</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="L9" s="7" t="s">
         <v>31</v>

</xml_diff>